<commit_message>
Updated data tracking sheet
</commit_message>
<xml_diff>
--- a/Notes/NERSC_data.xlsx
+++ b/Notes/NERSC_data.xlsx
@@ -1,44 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseyberger/Dropbox/Work/Projects/RotatingBosons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseyberger/Dropbox/Work/Projects/RotatingBosonsAMReX/nrrb/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D290B6-D4BC-094A-8F72-FE2140406E86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687FBC64-110E-B642-BF23-EF2498CFA6AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39740" yWindow="-2440" windowWidth="23720" windowHeight="15000" activeTab="1" xr2:uid="{C7F88351-C24A-5C48-8B03-33C49566896C}"/>
+    <workbookView xWindow="39740" yWindow="-2440" windowWidth="23720" windowHeight="15000" activeTab="2" xr2:uid="{C7F88351-C24A-5C48-8B03-33C49566896C}"/>
   </bookViews>
   <sheets>
     <sheet name="second tests Summer 2020" sheetId="1" r:id="rId1"/>
-    <sheet name="CL evol tests Summer 2020" sheetId="3" r:id="rId2"/>
+    <sheet name="Ka and eta tests 2020" sheetId="3" r:id="rId2"/>
+    <sheet name="Testing updated drift functions" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_beta">#N/A</definedName>
     <definedName name="Slicer_beta2">#N/A</definedName>
+    <definedName name="Slicer_beta21">#N/A</definedName>
     <definedName name="Slicer_dim">#N/A</definedName>
     <definedName name="Slicer_dim2">#N/A</definedName>
+    <definedName name="Slicer_dim21">#N/A</definedName>
     <definedName name="Slicer_eps">#N/A</definedName>
     <definedName name="Slicer_eps2">#N/A</definedName>
+    <definedName name="Slicer_eps21">#N/A</definedName>
     <definedName name="Slicer_lambda">#N/A</definedName>
     <definedName name="Slicer_lambda2">#N/A</definedName>
+    <definedName name="Slicer_lambda21">#N/A</definedName>
     <definedName name="Slicer_mu">#N/A</definedName>
     <definedName name="Slicer_mu2">#N/A</definedName>
+    <definedName name="Slicer_mu21">#N/A</definedName>
     <definedName name="Slicer_nL">#N/A</definedName>
     <definedName name="Slicer_nL2">#N/A</definedName>
+    <definedName name="Slicer_nL21">#N/A</definedName>
     <definedName name="Slicer_Nt">#N/A</definedName>
     <definedName name="Slicer_Nt2">#N/A</definedName>
+    <definedName name="Slicer_Nt21">#N/A</definedName>
     <definedName name="Slicer_Nx">#N/A</definedName>
     <definedName name="Slicer_Nx2">#N/A</definedName>
+    <definedName name="Slicer_Nx21">#N/A</definedName>
+    <definedName name="Slicer_Status">#N/A</definedName>
     <definedName name="Slicer_tL">#N/A</definedName>
     <definedName name="Slicer_tL2">#N/A</definedName>
+    <definedName name="Slicer_tL21">#N/A</definedName>
     <definedName name="Slicer_wtr">#N/A</definedName>
     <definedName name="Slicer_wtr2">#N/A</definedName>
+    <definedName name="Slicer_wtr21">#N/A</definedName>
     <definedName name="Slicer_wz">#N/A</definedName>
     <definedName name="Slicer_wz2">#N/A</definedName>
+    <definedName name="Slicer_wz21">#N/A</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +60,6 @@
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId3"/>
         <x14:slicerCache r:id="rId4"/>
         <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
@@ -69,6 +81,19 @@
         <x14:slicerCache r:id="rId22"/>
         <x14:slicerCache r:id="rId23"/>
         <x14:slicerCache r:id="rId24"/>
+        <x14:slicerCache r:id="rId25"/>
+        <x14:slicerCache r:id="rId26"/>
+        <x14:slicerCache r:id="rId27"/>
+        <x14:slicerCache r:id="rId28"/>
+        <x14:slicerCache r:id="rId29"/>
+        <x14:slicerCache r:id="rId30"/>
+        <x14:slicerCache r:id="rId31"/>
+        <x14:slicerCache r:id="rId32"/>
+        <x14:slicerCache r:id="rId33"/>
+        <x14:slicerCache r:id="rId34"/>
+        <x14:slicerCache r:id="rId35"/>
+        <x14:slicerCache r:id="rId36"/>
+        <x14:slicerCache r:id="rId37"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -79,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>dim</t>
   </si>
@@ -119,6 +144,12 @@
   <si>
     <t>wtr</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>to do</t>
+  </si>
 </sst>
 </file>
 
@@ -133,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -171,16 +208,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1078,8 +1119,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Nt 2">
@@ -1098,6 +1139,869 @@
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
               <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Nt 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1879600" y="38100"/>
+              <a:ext cx="1828800" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Nx 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191EFA6A-03D4-D948-94D0-11D3D293F5DC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Nx 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3721100" y="38100"/>
+              <a:ext cx="1828800" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>939800</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="beta 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C56C2F-E292-F443-B1A2-D05FD4A48573}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="beta 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5562600" y="25400"/>
+              <a:ext cx="1828800" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1003300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2374900</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="eps 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE404D17-C6EE-A646-B2FA-727A17DD1873}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="eps 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="38100" y="1003300"/>
+              <a:ext cx="1828800" cy="1371600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1003300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2374900</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="tL 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3AA5936-4EDC-5E40-8A7B-EE8DA9EC1A4E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="tL 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1879600" y="1003300"/>
+              <a:ext cx="1828800" cy="1371600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2387600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4216400</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="lambda 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F5BBED4-B64A-9641-AE3C-9DB38413D02D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="lambda 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5575300" y="2387600"/>
+              <a:ext cx="1828800" cy="1828800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4229100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="mu 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21D635F9-734E-FB48-875E-DECBFA69343D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="mu 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="38100" y="2400300"/>
+              <a:ext cx="1828800" cy="1828800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1003300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2374900</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="9" name="nL 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855F22E5-CBEE-E64A-9896-E50ED3FC8509}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="nL 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3721100" y="1003300"/>
+              <a:ext cx="1828800" cy="1371600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4229100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="10" name="wtr 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B125F9-6012-954F-85E1-A9CB6622C4CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wtr 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1879600" y="2400300"/>
+              <a:ext cx="1828800" cy="1828800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4229100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="11" name="wz 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655AA955-D425-D34F-86F1-A557AE58220E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wz 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3733800" y="2400300"/>
+              <a:ext cx="1828800" cy="1828800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="12" name="dim 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70094DA2-2A64-1043-91E7-63434254E1A3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="dim 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="25400" y="38100"/>
+              <a:ext cx="1828800" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>952500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Nt 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C146D143-7116-0B4A-9244-80DAC92668AB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Nt 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1160,10 +2064,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Nx 2">
+            <xdr:cNvPr id="3" name="Nx 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191EFA6A-03D4-D948-94D0-11D3D293F5DC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43EF1A7F-04EF-DF49-AE9E-215F35CA2C4C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1175,7 +2079,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Nx 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Nx 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1238,10 +2142,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="4" name="beta 2">
+            <xdr:cNvPr id="4" name="beta 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C56C2F-E292-F443-B1A2-D05FD4A48573}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{925AE2B6-61A1-DC48-9A3E-423005C0C353}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1253,7 +2157,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="beta 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="beta 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1316,10 +2220,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="5" name="eps 2">
+            <xdr:cNvPr id="5" name="eps 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE404D17-C6EE-A646-B2FA-727A17DD1873}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE67188B-4F80-7C42-B9BB-92EB0EE56B8B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1331,7 +2235,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="eps 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="eps 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1394,10 +2298,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="6" name="tL 2">
+            <xdr:cNvPr id="6" name="tL 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3AA5936-4EDC-5E40-8A7B-EE8DA9EC1A4E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A764B4BB-697F-424A-ACFF-3D793F8A5101}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1409,7 +2313,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="tL 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="tL 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1472,10 +2376,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="7" name="lambda 2">
+            <xdr:cNvPr id="7" name="lambda 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F5BBED4-B64A-9641-AE3C-9DB38413D02D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E10E8E-89E8-C644-BC04-E23C59A1CFC7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1487,7 +2391,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="lambda 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="lambda 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1550,10 +2454,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="8" name="mu 2">
+            <xdr:cNvPr id="8" name="mu 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21D635F9-734E-FB48-875E-DECBFA69343D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FD917FB-6FB7-3346-B10A-B11C2B375255}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1565,7 +2469,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="mu 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="mu 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1628,10 +2532,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="9" name="nL 2">
+            <xdr:cNvPr id="9" name="nL 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{855F22E5-CBEE-E64A-9896-E50ED3FC8509}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCA3DD26-11C5-F943-BA27-CE44D96E7920}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1643,7 +2547,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="nL 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="nL 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1706,10 +2610,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="10" name="wtr 2">
+            <xdr:cNvPr id="10" name="wtr 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B125F9-6012-954F-85E1-A9CB6622C4CF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C90454-8D9F-BF42-A66E-7CF43789F88A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1721,7 +2625,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wtr 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wtr 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1784,10 +2688,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="11" name="wz 2">
+            <xdr:cNvPr id="11" name="wz 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{655AA955-D425-D34F-86F1-A557AE58220E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CE0AB4-2556-B147-BB0D-F5904D669328}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1799,7 +2703,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wz 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="wz 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1862,10 +2766,10 @@
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="12" name="dim 2">
+            <xdr:cNvPr id="12" name="dim 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70094DA2-2A64-1043-91E7-63434254E1A3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2169675-5BFE-644E-A43D-03392BE19608}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1877,7 +2781,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="dim 2"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="dim 3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -1894,6 +2798,84 @@
             <a:xfrm>
               <a:off x="25400" y="38100"/>
               <a:ext cx="1828800" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a table slicer. Table slicers are not supported in this version of Excel.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2007 or earlier, the slicer can't be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1003300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2336800</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="13" name="Status">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACFFD63-BDE2-0F4B-A456-231BD662C6EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Status"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5588000" y="1003300"/>
+              <a:ext cx="1828800" cy="1333500"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2076,11 +3058,131 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache23.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Nt21" xr10:uid="{2CA9CC48-6BE0-0343-9F58-FB8ABDB9D508}" sourceName="Nt">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="2"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache24.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Nx21" xr10:uid="{37EBB05D-A80F-8643-BCF1-F63EBB165789}" sourceName="Nx">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="3"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache25.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_beta21" xr10:uid="{DFC79E4E-303D-F14C-836B-47F06BB623D9}" sourceName="beta">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="4"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache26.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_eps21" xr10:uid="{69EBA1BC-A510-CA42-8E9B-4C502F18E030}" sourceName="eps">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="6"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache27.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_tL21" xr10:uid="{648C3683-89CF-1B4E-B653-A72B9BA492AF}" sourceName="tL">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="15"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache28.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_lambda21" xr10:uid="{688C4DFA-3C1B-C74F-97DC-1184F16E2B9C}" sourceName="lambda">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="7"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache29.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_mu21" xr10:uid="{A8C8C77F-09D3-1C46-948C-E767850FEA7F}" sourceName="mu">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="9"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_beta" xr10:uid="{2A7A4145-B3C5-2F4B-9F46-26F6B2654A9B}" sourceName="beta">
   <extLst>
     <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
       <x15:tableSlicerCache tableId="1" column="4"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache30.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_nL21" xr10:uid="{09DB6476-E80E-544A-813E-92BC1F64DF54}" sourceName="nL">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="10"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache31.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_wtr21" xr10:uid="{826D6EF1-9972-FC47-B57F-781C37013D99}" sourceName="wtr">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="11"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache32.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_wz21" xr10:uid="{2B0FF85F-FD23-4840-AA06-21572A5EF7AD}" sourceName="wz">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="12"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache33.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_dim21" xr10:uid="{E9E8DA20-1E34-E647-882C-C225EF124289}" sourceName="dim">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="13"/>
+    </x:ext>
+  </extLst>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache34.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Status" xr10:uid="{F7067426-FD6E-E74E-BBB0-B7E23F9E7CE4}" sourceName="Status">
+  <extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{2F2917AC-EB37-4324-AD4E-5DD8C200BD13}">
+      <x15:tableSlicerCache tableId="2" column="1"/>
     </x:ext>
   </extLst>
 </slicerCacheDefinition>
@@ -2178,6 +3280,23 @@
 </slicers>
 </file>
 
+<file path=xl/slicers/slicer3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Nt 3" xr10:uid="{2E8E521C-AA62-F846-B9AF-1DF1E9120718}" cache="Slicer_Nt21" caption="Nt" columnCount="2" style="SlicerStyleDark5" rowHeight="251883"/>
+  <slicer name="Nx 3" xr10:uid="{63EB5C71-3B7C-1542-A9EF-68608181B8FA}" cache="Slicer_Nx21" caption="Nx" columnCount="2" style="SlicerStyleDark5" rowHeight="251883"/>
+  <slicer name="beta 3" xr10:uid="{130A1BA6-8F4C-E94F-B089-145BAE594103}" cache="Slicer_beta21" caption="beta" columnCount="2" style="SlicerStyleDark5" rowHeight="251883"/>
+  <slicer name="eps 3" xr10:uid="{82842C94-8FFA-AE41-A3B6-2C53CB592591}" cache="Slicer_eps21" caption="eps" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
+  <slicer name="tL 3" xr10:uid="{668104C1-281A-DB4E-8801-091A23E85320}" cache="Slicer_tL21" caption="tL" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
+  <slicer name="lambda 3" xr10:uid="{031CC79C-0609-AD43-89A7-2E8D87108609}" cache="Slicer_lambda21" caption="lambda" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
+  <slicer name="mu 3" xr10:uid="{CC8D1E13-03FB-EE4C-8359-53E8D0173547}" cache="Slicer_mu21" caption="mu" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
+  <slicer name="nL 3" xr10:uid="{82268951-E1BC-1543-80EE-C0A8A62DDE31}" cache="Slicer_nL21" caption="nL" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
+  <slicer name="wtr 3" xr10:uid="{D3950F56-F5E8-0E4A-A0FC-3450B2347223}" cache="Slicer_wtr21" caption="wtr" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
+  <slicer name="wz 3" xr10:uid="{4683A498-28A9-724D-AF4B-188B44595BD8}" cache="Slicer_wz21" caption="wz" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
+  <slicer name="dim 3" xr10:uid="{76213107-808A-394D-AE6D-69A3B429D8A9}" cache="Slicer_dim21" caption="dim" columnCount="2" style="SlicerStyleDark5" rowHeight="251883"/>
+  <slicer name="Status" xr10:uid="{A76CDC96-EA1C-B541-B99E-20878B68D244}" cache="Slicer_Status" caption="Status" style="SlicerStyleDark3" rowHeight="251883"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9255445C-339E-664C-9977-E8B9C9594D95}" name="Table1" displayName="Table1" ref="A2:M210" totalsRowShown="0">
   <autoFilter ref="A2:M210" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
@@ -2191,7 +3310,7 @@
     <tableColumn id="13" xr3:uid="{22E9BD1C-3607-C84A-B9C3-09EF4C849636}" name="dim"/>
     <tableColumn id="5" xr3:uid="{ED60D9CC-7445-4F4C-8606-26FCE3A4DFC4}" name="dt"/>
     <tableColumn id="6" xr3:uid="{514ED287-2983-4F43-B33E-3B3B6F2C9CC2}" name="eps"/>
-    <tableColumn id="15" xr3:uid="{CB7699E8-0D27-1542-8243-27A502B29BA4}" name="tL" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{CB7699E8-0D27-1542-8243-27A502B29BA4}" name="tL" dataDxfId="2">
       <calculatedColumnFormula>F3*K3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{6C4A9A27-40BC-5A40-A662-7EB7DE45021F}" name="lambda"/>
@@ -2206,25 +3325,59 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{72A91BAF-A2F9-5C4A-B568-69841A850942}" name="Table14" displayName="Table14" ref="A2:M3" totalsRowShown="0">
-  <autoFilter ref="A2:M3" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
-  <sortState ref="A3:M3">
-    <sortCondition descending="1" ref="F2:F3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{72A91BAF-A2F9-5C4A-B568-69841A850942}" name="Table14" displayName="Table14" ref="A2:M8" totalsRowShown="0">
+  <autoFilter ref="A2:M8" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
+  <sortState ref="A3:M7">
+    <sortCondition descending="1" ref="F2:F7"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="2" xr3:uid="{5DCA735E-4935-5349-9F2B-989C0CD308D6}" name="Nt"/>
     <tableColumn id="3" xr3:uid="{299EDB1B-26A9-F54B-9A70-ADC2C88BAA8C}" name="Nx"/>
-    <tableColumn id="4" xr3:uid="{04A0970B-CA74-3B42-8785-5D50912B4F51}" name="beta"/>
+    <tableColumn id="4" xr3:uid="{04A0970B-CA74-3B42-8785-5D50912B4F51}" name="beta">
+      <calculatedColumnFormula>Table14[Nt]*Table14[dt]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="13" xr3:uid="{0B1B7D8E-4406-6C4F-A263-23638E63B46E}" name="dim"/>
     <tableColumn id="5" xr3:uid="{1A259FEB-F025-D64D-AFA6-36E762874C99}" name="dt"/>
     <tableColumn id="6" xr3:uid="{60D69032-318B-DD4F-8B77-61F56A3EEFC6}" name="eps"/>
-    <tableColumn id="15" xr3:uid="{87C8FE9A-46E3-FC47-B4FF-A966F659F135}" name="tL" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{87C8FE9A-46E3-FC47-B4FF-A966F659F135}" name="tL" dataDxfId="1">
+      <calculatedColumnFormula>Table14[eps]*Table14[nL]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="7" xr3:uid="{69862EFB-DD6A-804C-AEE4-AA804409710D}" name="lambda"/>
     <tableColumn id="8" xr3:uid="{34EEFCD8-6E6C-B941-B830-947C393A2051}" name="m"/>
     <tableColumn id="9" xr3:uid="{C8317EDD-6D17-C147-BBC5-36979C4C9EF9}" name="mu"/>
     <tableColumn id="10" xr3:uid="{3BF3F386-9BD2-F143-9254-5B8770C46AC7}" name="nL"/>
     <tableColumn id="11" xr3:uid="{E3B3632B-2679-A345-9ADE-56E6AEDA466D}" name="wtr"/>
     <tableColumn id="12" xr3:uid="{A99D388B-0483-ED40-9EB6-D3D5279B2CD2}" name="wz"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81393967-7F43-8646-B237-74462FC7A100}" name="Table143" displayName="Table143" ref="A2:N14" totalsRowShown="0">
+  <autoFilter ref="A2:N14" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
+  <sortState ref="A3:M7">
+    <sortCondition descending="1" ref="F2:F7"/>
+  </sortState>
+  <tableColumns count="14">
+    <tableColumn id="2" xr3:uid="{36E8B953-B85F-D54C-8F14-1853981F80E3}" name="Nt"/>
+    <tableColumn id="3" xr3:uid="{6F7F14F3-F561-4F4A-8AFF-82DBCCF6B0E4}" name="Nx"/>
+    <tableColumn id="4" xr3:uid="{53641338-5B42-034C-A29C-CE28C106D802}" name="beta">
+      <calculatedColumnFormula>Table143[Nt]*Table143[dt]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{0107E2E5-AC28-504C-8B60-CF83C105EED2}" name="dim"/>
+    <tableColumn id="5" xr3:uid="{1A0B1BB8-AEC6-4F4B-8FFA-E9B272B6F2D4}" name="dt"/>
+    <tableColumn id="6" xr3:uid="{F05E41FD-F569-304E-8F07-1BE0CF262EA8}" name="eps"/>
+    <tableColumn id="15" xr3:uid="{79406169-9E1C-7D43-A9F0-1B5EFA66A9F5}" name="tL" dataDxfId="0">
+      <calculatedColumnFormula>Table143[eps]*Table143[nL]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{1CA6FD7B-F5D0-7640-A8F9-6BEF36D6CFF1}" name="lambda"/>
+    <tableColumn id="8" xr3:uid="{374DE6DB-41FD-B04A-B3FC-A929CF84AB2D}" name="m"/>
+    <tableColumn id="9" xr3:uid="{51ECF7F4-1580-E040-8172-0AB1B4FF1355}" name="mu"/>
+    <tableColumn id="10" xr3:uid="{A24D337A-ED73-DF46-8FB1-CCCBDAB3DC2E}" name="nL"/>
+    <tableColumn id="11" xr3:uid="{F0E7CE1E-F45F-3940-A7C4-D84D501A970F}" name="wtr"/>
+    <tableColumn id="12" xr3:uid="{A0FFFA32-42F8-B34B-8FC9-AC2E65B291E3}" name="wz"/>
+    <tableColumn id="1" xr3:uid="{F38B9F1E-F870-944E-AF61-A6943BD5899A}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11331,10 +12484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD2B83F-2D7B-A64D-98F4-965259993735}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11379,6 +12532,887 @@
       </c>
       <c r="M2" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="F3">
+        <v>0.01</v>
+      </c>
+      <c r="G3">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>-0.1</v>
+      </c>
+      <c r="K3">
+        <v>10000</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>160</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0.05</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>-0.2</v>
+      </c>
+      <c r="K4">
+        <v>10000</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10000</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="F6">
+        <v>1E-3</v>
+      </c>
+      <c r="G6">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>-0.1</v>
+      </c>
+      <c r="K6">
+        <v>100000</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>160</v>
+      </c>
+      <c r="B7">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7">
+        <v>1E-3</v>
+      </c>
+      <c r="G7">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>-0.2</v>
+      </c>
+      <c r="K7">
+        <v>100000</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>160</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <f>Table14[Nt]*Table14[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>1E-3</v>
+      </c>
+      <c r="G8">
+        <f>Table14[eps]*Table14[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>100000</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
+      <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41128F09-A9EA-234F-A0B4-81898E178F15}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="338" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0.05</v>
+      </c>
+      <c r="F3">
+        <v>0.01</v>
+      </c>
+      <c r="G3">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>-0.1</v>
+      </c>
+      <c r="K3">
+        <v>10000</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>160</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0.05</v>
+      </c>
+      <c r="F4">
+        <v>0.01</v>
+      </c>
+      <c r="G4">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>-0.2</v>
+      </c>
+      <c r="K4">
+        <v>10000</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>160</v>
+      </c>
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0.05</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>10000</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0.05</v>
+      </c>
+      <c r="F6">
+        <v>1E-3</v>
+      </c>
+      <c r="G6">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>-0.1</v>
+      </c>
+      <c r="K6">
+        <v>100000</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>160</v>
+      </c>
+      <c r="B7">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7">
+        <v>1E-3</v>
+      </c>
+      <c r="G7">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>-0.2</v>
+      </c>
+      <c r="K7">
+        <v>100000</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>160</v>
+      </c>
+      <c r="B8">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>1E-3</v>
+      </c>
+      <c r="G8">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>100000</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>160</v>
+      </c>
+      <c r="B9">
+        <v>41</v>
+      </c>
+      <c r="C9">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <v>0.01</v>
+      </c>
+      <c r="G9">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>-0.3</v>
+      </c>
+      <c r="K9">
+        <v>10000</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0.05</v>
+      </c>
+      <c r="F10">
+        <v>0.01</v>
+      </c>
+      <c r="G10">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>-0.5</v>
+      </c>
+      <c r="K10">
+        <v>10000</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>160</v>
+      </c>
+      <c r="B11">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0.05</v>
+      </c>
+      <c r="F11">
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>-1</v>
+      </c>
+      <c r="K11">
+        <v>10000</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>160</v>
+      </c>
+      <c r="B12">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0.05</v>
+      </c>
+      <c r="F12">
+        <v>1E-3</v>
+      </c>
+      <c r="G12">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>-0.3</v>
+      </c>
+      <c r="K12">
+        <v>100000</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>160</v>
+      </c>
+      <c r="B13">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0.05</v>
+      </c>
+      <c r="F13">
+        <v>1E-3</v>
+      </c>
+      <c r="G13">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>-0.5</v>
+      </c>
+      <c r="K13">
+        <v>100000</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>160</v>
+      </c>
+      <c r="B14">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0.05</v>
+      </c>
+      <c r="F14">
+        <v>1E-3</v>
+      </c>
+      <c r="G14">
+        <f>Table143[eps]*Table143[nL]</f>
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>-1</v>
+      </c>
+      <c r="K14">
+        <v>100000</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet with new jobs submitted
</commit_message>
<xml_diff>
--- a/Notes/NERSC_data.xlsx
+++ b/Notes/NERSC_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseyberger/Dropbox/Work/Projects/RotatingBosonsAMReX/nrrb/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687FBC64-110E-B642-BF23-EF2498CFA6AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC0A429-54BB-B342-90FD-75A781EFF321}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39740" yWindow="-2440" windowWidth="23720" windowHeight="15000" activeTab="2" xr2:uid="{C7F88351-C24A-5C48-8B03-33C49566896C}"/>
+    <workbookView xWindow="33140" yWindow="-2440" windowWidth="24640" windowHeight="14740" activeTab="2" xr2:uid="{C7F88351-C24A-5C48-8B03-33C49566896C}"/>
   </bookViews>
   <sheets>
     <sheet name="second tests Summer 2020" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
   <si>
     <t>dim</t>
   </si>
@@ -148,20 +148,35 @@
     <t>Status</t>
   </si>
   <si>
-    <t>to do</t>
+    <t>jobid</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -208,19 +223,229 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1982,8 +2207,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Nt 3">
@@ -2006,7 +2231,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2060,8 +2285,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Nx 3">
@@ -2084,7 +2309,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2138,8 +2363,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>939800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="beta 3">
@@ -2162,7 +2387,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2216,8 +2441,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2374900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="eps 3">
@@ -2240,7 +2465,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2294,8 +2519,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2374900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="tL 3">
@@ -2318,7 +2543,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2372,8 +2597,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>4216400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="lambda 3">
@@ -2396,7 +2621,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2450,8 +2675,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>4229100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="8" name="mu 3">
@@ -2474,7 +2699,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2528,8 +2753,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2374900</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="9" name="nL 3">
@@ -2552,7 +2777,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2606,8 +2831,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>4229100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="10" name="wtr 3">
@@ -2630,7 +2855,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2684,8 +2909,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>4229100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="11" name="wz 3">
@@ -2708,7 +2933,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2762,8 +2987,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="12" name="dim 3">
@@ -2786,7 +3011,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2840,8 +3065,8 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>2336800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="13" name="Status">
@@ -2864,7 +3089,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3288,12 +3513,12 @@
   <slicer name="eps 3" xr10:uid="{82842C94-8FFA-AE41-A3B6-2C53CB592591}" cache="Slicer_eps21" caption="eps" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
   <slicer name="tL 3" xr10:uid="{668104C1-281A-DB4E-8801-091A23E85320}" cache="Slicer_tL21" caption="tL" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
   <slicer name="lambda 3" xr10:uid="{031CC79C-0609-AD43-89A7-2E8D87108609}" cache="Slicer_lambda21" caption="lambda" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
-  <slicer name="mu 3" xr10:uid="{CC8D1E13-03FB-EE4C-8359-53E8D0173547}" cache="Slicer_mu21" caption="mu" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
+  <slicer name="mu 3" xr10:uid="{CC8D1E13-03FB-EE4C-8359-53E8D0173547}" cache="Slicer_mu21" caption="mu" startItem="2" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
   <slicer name="nL 3" xr10:uid="{82268951-E1BC-1543-80EE-C0A8A62DDE31}" cache="Slicer_nL21" caption="nL" columnCount="2" style="SlicerStyleDark2" rowHeight="251883"/>
   <slicer name="wtr 3" xr10:uid="{D3950F56-F5E8-0E4A-A0FC-3450B2347223}" cache="Slicer_wtr21" caption="wtr" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
   <slicer name="wz 3" xr10:uid="{4683A498-28A9-724D-AF4B-188B44595BD8}" cache="Slicer_wz21" caption="wz" columnCount="2" style="SlicerStyleDark6" rowHeight="251883"/>
   <slicer name="dim 3" xr10:uid="{76213107-808A-394D-AE6D-69A3B429D8A9}" cache="Slicer_dim21" caption="dim" columnCount="2" style="SlicerStyleDark5" rowHeight="251883"/>
-  <slicer name="Status" xr10:uid="{A76CDC96-EA1C-B541-B99E-20878B68D244}" cache="Slicer_Status" caption="Status" style="SlicerStyleDark3" rowHeight="251883"/>
+  <slicer name="Status" xr10:uid="{A76CDC96-EA1C-B541-B99E-20878B68D244}" cache="Slicer_Status" caption="Status" style="SlicerStyleOther1" rowHeight="251883"/>
 </slicers>
 </file>
 
@@ -3310,7 +3535,7 @@
     <tableColumn id="13" xr3:uid="{22E9BD1C-3607-C84A-B9C3-09EF4C849636}" name="dim"/>
     <tableColumn id="5" xr3:uid="{ED60D9CC-7445-4F4C-8606-26FCE3A4DFC4}" name="dt"/>
     <tableColumn id="6" xr3:uid="{514ED287-2983-4F43-B33E-3B3B6F2C9CC2}" name="eps"/>
-    <tableColumn id="15" xr3:uid="{CB7699E8-0D27-1542-8243-27A502B29BA4}" name="tL" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{CB7699E8-0D27-1542-8243-27A502B29BA4}" name="tL" dataDxfId="17">
       <calculatedColumnFormula>F3*K3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{6C4A9A27-40BC-5A40-A662-7EB7DE45021F}" name="lambda"/>
@@ -3339,7 +3564,7 @@
     <tableColumn id="13" xr3:uid="{0B1B7D8E-4406-6C4F-A263-23638E63B46E}" name="dim"/>
     <tableColumn id="5" xr3:uid="{1A259FEB-F025-D64D-AFA6-36E762874C99}" name="dt"/>
     <tableColumn id="6" xr3:uid="{60D69032-318B-DD4F-8B77-61F56A3EEFC6}" name="eps"/>
-    <tableColumn id="15" xr3:uid="{87C8FE9A-46E3-FC47-B4FF-A966F659F135}" name="tL" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{87C8FE9A-46E3-FC47-B4FF-A966F659F135}" name="tL" dataDxfId="16">
       <calculatedColumnFormula>Table14[eps]*Table14[nL]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{69862EFB-DD6A-804C-AEE4-AA804409710D}" name="lambda"/>
@@ -3354,30 +3579,31 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81393967-7F43-8646-B237-74462FC7A100}" name="Table143" displayName="Table143" ref="A2:N14" totalsRowShown="0">
-  <autoFilter ref="A2:N14" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81393967-7F43-8646-B237-74462FC7A100}" name="Table143" displayName="Table143" ref="A2:O46" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A2:O46" xr:uid="{B48ACC55-F3CD-9A4B-8B20-097CD0960467}"/>
   <sortState ref="A3:M7">
     <sortCondition descending="1" ref="F2:F7"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="2" xr3:uid="{36E8B953-B85F-D54C-8F14-1853981F80E3}" name="Nt"/>
-    <tableColumn id="3" xr3:uid="{6F7F14F3-F561-4F4A-8AFF-82DBCCF6B0E4}" name="Nx"/>
-    <tableColumn id="4" xr3:uid="{53641338-5B42-034C-A29C-CE28C106D802}" name="beta">
+  <tableColumns count="15">
+    <tableColumn id="2" xr3:uid="{36E8B953-B85F-D54C-8F14-1853981F80E3}" name="Nt" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{6F7F14F3-F561-4F4A-8AFF-82DBCCF6B0E4}" name="Nx" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{53641338-5B42-034C-A29C-CE28C106D802}" name="beta" dataDxfId="13">
       <calculatedColumnFormula>Table143[Nt]*Table143[dt]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0107E2E5-AC28-504C-8B60-CF83C105EED2}" name="dim"/>
-    <tableColumn id="5" xr3:uid="{1A0B1BB8-AEC6-4F4B-8FFA-E9B272B6F2D4}" name="dt"/>
-    <tableColumn id="6" xr3:uid="{F05E41FD-F569-304E-8F07-1BE0CF262EA8}" name="eps"/>
-    <tableColumn id="15" xr3:uid="{79406169-9E1C-7D43-A9F0-1B5EFA66A9F5}" name="tL" dataDxfId="0">
+    <tableColumn id="13" xr3:uid="{0107E2E5-AC28-504C-8B60-CF83C105EED2}" name="dim" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{1A0B1BB8-AEC6-4F4B-8FFA-E9B272B6F2D4}" name="dt" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{F05E41FD-F569-304E-8F07-1BE0CF262EA8}" name="eps" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{79406169-9E1C-7D43-A9F0-1B5EFA66A9F5}" name="tL" dataDxfId="9">
       <calculatedColumnFormula>Table143[eps]*Table143[nL]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1CA6FD7B-F5D0-7640-A8F9-6BEF36D6CFF1}" name="lambda"/>
-    <tableColumn id="8" xr3:uid="{374DE6DB-41FD-B04A-B3FC-A929CF84AB2D}" name="m"/>
-    <tableColumn id="9" xr3:uid="{51ECF7F4-1580-E040-8172-0AB1B4FF1355}" name="mu"/>
-    <tableColumn id="10" xr3:uid="{A24D337A-ED73-DF46-8FB1-CCCBDAB3DC2E}" name="nL"/>
-    <tableColumn id="11" xr3:uid="{F0E7CE1E-F45F-3940-A7C4-D84D501A970F}" name="wtr"/>
-    <tableColumn id="12" xr3:uid="{A0FFFA32-42F8-B34B-8FC9-AC2E65B291E3}" name="wz"/>
-    <tableColumn id="1" xr3:uid="{F38B9F1E-F870-944E-AF61-A6943BD5899A}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{1CA6FD7B-F5D0-7640-A8F9-6BEF36D6CFF1}" name="lambda" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{374DE6DB-41FD-B04A-B3FC-A929CF84AB2D}" name="m" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{51ECF7F4-1580-E040-8172-0AB1B4FF1355}" name="mu" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{A24D337A-ED73-DF46-8FB1-CCCBDAB3DC2E}" name="nL" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{F0E7CE1E-F45F-3940-A7C4-D84D501A970F}" name="wtr" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{A0FFFA32-42F8-B34B-8FC9-AC2E65B291E3}" name="wz" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{F7749B94-AAE2-624E-B419-89C82CDEE3AD}" name="jobid" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F38B9F1E-F870-944E-AF61-A6943BD5899A}" name="Status" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12810,16 +13036,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41128F09-A9EA-234F-A0B4-81898E178F15}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="338" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="338" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -12859,560 +13088,2167 @@
       <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>160</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>160</v>
+      </c>
+      <c r="B3" s="5">
         <v>41</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>0.05</v>
-      </c>
-      <c r="F3">
-        <v>0.01</v>
-      </c>
-      <c r="G3">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G3" s="5">
         <v>100</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>-1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>34724117</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>160</v>
+      </c>
+      <c r="B4" s="5">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="5">
+        <v>100</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>34724098</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>160</v>
+      </c>
+      <c r="B5" s="5">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>100</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>34724087</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>160</v>
+      </c>
+      <c r="B6" s="5">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>100</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>-0.7</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
+        <v>34724083</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>160</v>
+      </c>
+      <c r="B7" s="5">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="5">
+        <v>100</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7">
+        <v>34724055</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>160</v>
+      </c>
+      <c r="B8" s="5">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="5">
+        <v>100</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="7">
+        <v>34724050</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>160</v>
+      </c>
+      <c r="B9" s="5">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G9" s="5">
+        <v>100</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="7">
+        <v>34724036</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>160</v>
+      </c>
+      <c r="B10" s="5">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G10" s="5">
+        <v>100</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7">
+        <v>34724029</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>160</v>
+      </c>
+      <c r="B11" s="5">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="5">
+        <v>100</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="7">
+        <v>34724004</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>160</v>
+      </c>
+      <c r="B12" s="5">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5">
         <v>-0.1</v>
       </c>
-      <c r="K3">
-        <v>10000</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>160</v>
-      </c>
-      <c r="B4">
+      <c r="K12" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="7">
+        <v>34723955</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>160</v>
+      </c>
+      <c r="B13" s="5">
         <v>41</v>
       </c>
-      <c r="C4">
+      <c r="C13" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>0.05</v>
-      </c>
-      <c r="F4">
-        <v>0.01</v>
-      </c>
-      <c r="G4">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G13" s="5">
         <v>100</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="7">
+        <v>34724120</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>160</v>
+      </c>
+      <c r="B14" s="5">
+        <v>41</v>
+      </c>
+      <c r="C14" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>100</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="7">
+        <v>34723901</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>160</v>
+      </c>
+      <c r="B15" s="5">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>100</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="K15" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>34723896</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>160</v>
+      </c>
+      <c r="B16" s="5">
+        <v>41</v>
+      </c>
+      <c r="C16" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>100</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="K16" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <v>34723893</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>160</v>
+      </c>
+      <c r="B17" s="5">
+        <v>41</v>
+      </c>
+      <c r="C17" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G17" s="5">
+        <v>100</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
+      <c r="J17" s="5">
+        <v>-0.7</v>
+      </c>
+      <c r="K17" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>34723874</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>160</v>
+      </c>
+      <c r="B18" s="5">
+        <v>41</v>
+      </c>
+      <c r="C18" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G18" s="5">
+        <v>100</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="K18" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="7">
+        <v>34723845</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>160</v>
+      </c>
+      <c r="B19" s="5">
+        <v>41</v>
+      </c>
+      <c r="C19" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F19" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G19" s="5">
+        <v>100</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>1</v>
+      </c>
+      <c r="J19" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="K19" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="7">
+        <v>34723840</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>160</v>
+      </c>
+      <c r="B20" s="5">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F20" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G20" s="5">
+        <v>100</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K20" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>34723779</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>160</v>
+      </c>
+      <c r="B21" s="5">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G21" s="5">
+        <v>100</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="K21" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L21" s="5">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7">
+        <v>34723760</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>160</v>
+      </c>
+      <c r="B22" s="5">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G22" s="5">
+        <v>100</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5">
         <v>-0.2</v>
       </c>
-      <c r="K4">
-        <v>10000</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>160</v>
-      </c>
-      <c r="B5">
+      <c r="K22" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="7">
+        <v>34723742</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>160</v>
+      </c>
+      <c r="B23" s="5">
         <v>41</v>
       </c>
-      <c r="C5">
+      <c r="C23" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>0.05</v>
-      </c>
-      <c r="F5">
-        <v>0.01</v>
-      </c>
-      <c r="G5">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F23" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G23" s="5">
         <v>100</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>10000</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>160</v>
-      </c>
-      <c r="B6">
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="7">
+        <v>34723720</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>160</v>
+      </c>
+      <c r="B24" s="5">
         <v>41</v>
       </c>
-      <c r="C6">
+      <c r="C24" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>0.05</v>
-      </c>
-      <c r="F6">
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
         <v>1E-3</v>
       </c>
-      <c r="G6">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="G24" s="5">
         <v>100</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="7">
+        <v>34723907</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>160</v>
+      </c>
+      <c r="B25" s="5">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F25" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G25" s="5">
+        <v>100</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5">
+        <v>-1</v>
+      </c>
+      <c r="K25" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0</v>
+      </c>
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+      <c r="N25" s="7">
+        <v>34724283</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>160</v>
+      </c>
+      <c r="B26" s="5">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G26" s="5">
+        <v>100</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="K26" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L26" s="5">
+        <v>0</v>
+      </c>
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
+        <v>34724271</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>160</v>
+      </c>
+      <c r="B27" s="5">
+        <v>21</v>
+      </c>
+      <c r="C27" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G27" s="5">
+        <v>100</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="K27" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="7">
+        <v>34724237</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>160</v>
+      </c>
+      <c r="B28" s="5">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F28" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G28" s="5">
+        <v>100</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5">
+        <v>-0.7</v>
+      </c>
+      <c r="K28" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L28" s="5">
+        <v>0</v>
+      </c>
+      <c r="M28" s="5">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>34724222</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>160</v>
+      </c>
+      <c r="B29" s="5">
+        <v>21</v>
+      </c>
+      <c r="C29" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F29" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G29" s="5">
+        <v>100</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="K29" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7">
+        <v>34724212</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>160</v>
+      </c>
+      <c r="B30" s="5">
+        <v>21</v>
+      </c>
+      <c r="C30" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G30" s="5">
+        <v>100</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="K30" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L30" s="5">
+        <v>0</v>
+      </c>
+      <c r="M30" s="5">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7">
+        <v>34724191</v>
+      </c>
+      <c r="O30" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>160</v>
+      </c>
+      <c r="B31" s="5">
+        <v>21</v>
+      </c>
+      <c r="C31" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G31" s="5">
+        <v>100</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K31" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7">
+        <v>34724174</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>160</v>
+      </c>
+      <c r="B32" s="5">
+        <v>21</v>
+      </c>
+      <c r="C32" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G32" s="5">
+        <v>100</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>1</v>
+      </c>
+      <c r="J32" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="K32" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L32" s="5">
+        <v>0</v>
+      </c>
+      <c r="M32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7">
+        <v>34724169</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>160</v>
+      </c>
+      <c r="B33" s="5">
+        <v>21</v>
+      </c>
+      <c r="C33" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G33" s="5">
+        <v>100</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5">
+        <v>-0.2</v>
+      </c>
+      <c r="K33" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L33" s="5">
+        <v>0</v>
+      </c>
+      <c r="M33" s="5">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7">
+        <v>34724145</v>
+      </c>
+      <c r="O33" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>160</v>
+      </c>
+      <c r="B34" s="5">
+        <v>21</v>
+      </c>
+      <c r="C34" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F34" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G34" s="5">
+        <v>100</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5">
         <v>-0.1</v>
       </c>
-      <c r="K6">
+      <c r="K34" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L34" s="5">
+        <v>0</v>
+      </c>
+      <c r="M34" s="5">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7">
+        <v>34724141</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>160</v>
+      </c>
+      <c r="B35" s="5">
+        <v>21</v>
+      </c>
+      <c r="C35" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F35" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-4</v>
+      </c>
+      <c r="G35" s="5">
+        <v>100</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0</v>
+      </c>
+      <c r="K35" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="L35" s="5">
+        <v>0</v>
+      </c>
+      <c r="M35" s="5">
+        <v>0</v>
+      </c>
+      <c r="N35" s="7">
+        <v>34724296</v>
+      </c>
+      <c r="O35" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>160</v>
+      </c>
+      <c r="B36" s="5">
+        <v>21</v>
+      </c>
+      <c r="C36" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F36" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G36" s="5">
+        <v>100</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5">
+        <v>-1</v>
+      </c>
+      <c r="K36" s="5">
         <v>100000</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>160</v>
-      </c>
-      <c r="B7">
-        <v>41</v>
-      </c>
-      <c r="C7">
+      <c r="L36" s="5">
+        <v>0</v>
+      </c>
+      <c r="M36" s="5">
+        <v>0</v>
+      </c>
+      <c r="N36" s="7">
+        <v>34703540</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>160</v>
+      </c>
+      <c r="B37" s="5">
+        <v>21</v>
+      </c>
+      <c r="C37" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>0.05</v>
-      </c>
-      <c r="F7">
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F37" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
         <v>1E-3</v>
       </c>
-      <c r="G7">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="G37" s="5">
         <v>100</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>1</v>
+      </c>
+      <c r="J37" s="5">
+        <v>-0.9</v>
+      </c>
+      <c r="K37" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L37" s="5">
+        <v>0</v>
+      </c>
+      <c r="M37" s="5">
+        <v>0</v>
+      </c>
+      <c r="N37" s="7">
+        <v>34703531</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>160</v>
+      </c>
+      <c r="B38" s="5">
+        <v>21</v>
+      </c>
+      <c r="C38" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G38" s="5">
+        <v>100</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1</v>
+      </c>
+      <c r="J38" s="5">
+        <v>-0.8</v>
+      </c>
+      <c r="K38" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L38" s="5">
+        <v>0</v>
+      </c>
+      <c r="M38" s="5">
+        <v>0</v>
+      </c>
+      <c r="N38" s="7">
+        <v>34703528</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>160</v>
+      </c>
+      <c r="B39" s="5">
+        <v>21</v>
+      </c>
+      <c r="C39" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D39" s="5">
+        <v>2</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F39" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G39" s="5">
+        <v>100</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5">
+        <v>-0.7</v>
+      </c>
+      <c r="K39" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0</v>
+      </c>
+      <c r="M39" s="5">
+        <v>0</v>
+      </c>
+      <c r="N39" s="7">
+        <v>34703498</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>160</v>
+      </c>
+      <c r="B40" s="5">
+        <v>21</v>
+      </c>
+      <c r="C40" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D40" s="5">
+        <v>2</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F40" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G40" s="5">
+        <v>100</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5">
+        <v>-0.6</v>
+      </c>
+      <c r="K40" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L40" s="5">
+        <v>0</v>
+      </c>
+      <c r="M40" s="5">
+        <v>0</v>
+      </c>
+      <c r="N40" s="7">
+        <v>34703482</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>160</v>
+      </c>
+      <c r="B41" s="5">
+        <v>21</v>
+      </c>
+      <c r="C41" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D41" s="5">
+        <v>2</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F41" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G41" s="5">
+        <v>100</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="K41" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5">
+        <v>0</v>
+      </c>
+      <c r="N41" s="7">
+        <v>34703309</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>160</v>
+      </c>
+      <c r="B42" s="5">
+        <v>21</v>
+      </c>
+      <c r="C42" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D42" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F42" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G42" s="5">
+        <v>100</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5">
+        <v>-0.4</v>
+      </c>
+      <c r="K42" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L42" s="5">
+        <v>0</v>
+      </c>
+      <c r="M42" s="5">
+        <v>0</v>
+      </c>
+      <c r="N42" s="7">
+        <v>34703302</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>160</v>
+      </c>
+      <c r="B43" s="5">
+        <v>21</v>
+      </c>
+      <c r="C43" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D43" s="5">
+        <v>2</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F43" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G43" s="5">
+        <v>100</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5">
+        <v>-0.3</v>
+      </c>
+      <c r="K43" s="5">
+        <v>100000</v>
+      </c>
+      <c r="L43" s="5">
+        <v>0</v>
+      </c>
+      <c r="M43" s="5">
+        <v>0</v>
+      </c>
+      <c r="N43" s="7">
+        <v>34703297</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>160</v>
+      </c>
+      <c r="B44" s="5">
+        <v>21</v>
+      </c>
+      <c r="C44" s="5">
+        <f>Table143[Nt]*Table143[dt]</f>
+        <v>8</v>
+      </c>
+      <c r="D44" s="5">
+        <v>2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F44" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G44" s="5">
+        <v>100</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5">
         <v>-0.2</v>
       </c>
-      <c r="K7">
+      <c r="K44" s="5">
         <v>100000</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>160</v>
-      </c>
-      <c r="B8">
-        <v>41</v>
-      </c>
-      <c r="C8">
+      <c r="L44" s="5">
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <v>0</v>
+      </c>
+      <c r="N44" s="7">
+        <v>34703250</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>160</v>
+      </c>
+      <c r="B45" s="5">
+        <v>21</v>
+      </c>
+      <c r="C45" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>0.05</v>
-      </c>
-      <c r="F8">
+      <c r="D45" s="5">
+        <v>2</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F45" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
         <v>1E-3</v>
       </c>
-      <c r="G8">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="G45" s="5">
         <v>100</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="5">
+        <v>-0.1</v>
+      </c>
+      <c r="K45" s="5">
         <v>100000</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>160</v>
-      </c>
-      <c r="B9">
-        <v>41</v>
-      </c>
-      <c r="C9">
+      <c r="L45" s="5">
+        <v>0</v>
+      </c>
+      <c r="M45" s="5">
+        <v>0</v>
+      </c>
+      <c r="N45" s="7">
+        <v>34703225</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>160</v>
+      </c>
+      <c r="B46" s="5">
+        <v>21</v>
+      </c>
+      <c r="C46" s="5">
         <f>Table143[Nt]*Table143[dt]</f>
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>0.05</v>
-      </c>
-      <c r="F9">
-        <v>0.01</v>
-      </c>
-      <c r="G9">
-        <f>Table143[eps]*Table143[nL]</f>
+      <c r="D46" s="5">
+        <v>2</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F46" s="5">
+        <f>Table143[[#This Row],[tL]]/Table143[[#This Row],[nL]]</f>
+        <v>1E-3</v>
+      </c>
+      <c r="G46" s="5">
         <v>100</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>-0.3</v>
-      </c>
-      <c r="K9">
-        <v>10000</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>160</v>
-      </c>
-      <c r="B10">
-        <v>41</v>
-      </c>
-      <c r="C10">
-        <f>Table143[Nt]*Table143[dt]</f>
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10">
-        <v>0.05</v>
-      </c>
-      <c r="F10">
-        <v>0.01</v>
-      </c>
-      <c r="G10">
-        <f>Table143[eps]*Table143[nL]</f>
-        <v>100</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>-0.5</v>
-      </c>
-      <c r="K10">
-        <v>10000</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>160</v>
-      </c>
-      <c r="B11">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <f>Table143[Nt]*Table143[dt]</f>
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>0.05</v>
-      </c>
-      <c r="F11">
-        <v>0.01</v>
-      </c>
-      <c r="G11">
-        <f>Table143[eps]*Table143[nL]</f>
-        <v>100</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>-1</v>
-      </c>
-      <c r="K11">
-        <v>10000</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>160</v>
-      </c>
-      <c r="B12">
-        <v>41</v>
-      </c>
-      <c r="C12">
-        <f>Table143[Nt]*Table143[dt]</f>
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>0.05</v>
-      </c>
-      <c r="F12">
-        <v>1E-3</v>
-      </c>
-      <c r="G12">
-        <f>Table143[eps]*Table143[nL]</f>
-        <v>100</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>-0.3</v>
-      </c>
-      <c r="K12">
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>1</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
         <v>100000</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>160</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <f>Table143[Nt]*Table143[dt]</f>
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>0.05</v>
-      </c>
-      <c r="F13">
-        <v>1E-3</v>
-      </c>
-      <c r="G13">
-        <f>Table143[eps]*Table143[nL]</f>
-        <v>100</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>-0.5</v>
-      </c>
-      <c r="K13">
-        <v>100000</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>160</v>
-      </c>
-      <c r="B14">
-        <v>41</v>
-      </c>
-      <c r="C14">
-        <f>Table143[Nt]*Table143[dt]</f>
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>0.05</v>
-      </c>
-      <c r="F14">
-        <v>1E-3</v>
-      </c>
-      <c r="G14">
-        <f>Table143[eps]*Table143[nL]</f>
-        <v>100</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>-1</v>
-      </c>
-      <c r="K14">
-        <v>100000</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>14</v>
+      <c r="L46" s="5">
+        <v>0</v>
+      </c>
+      <c r="M46" s="5">
+        <v>0</v>
+      </c>
+      <c r="N46" s="7">
+        <v>34703546</v>
+      </c>
+      <c r="O46" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>